<commit_message>
Update report xlsx file
</commit_message>
<xml_diff>
--- a/project/spam_mail_detection/주간&일일보고.xlsx
+++ b/project/spam_mail_detection/주간&일일보고.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramie\OneDrive\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramie\OneDrive\Documents\learn_programming\project\spam_mail_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CEBD8E-E0B9-44CB-8697-608474EEEE12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749F431A-6FFD-466C-88CD-82A8667DDCE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11220" windowHeight="5208" xr2:uid="{03C89AB5-3466-4C93-B69B-4E1CD49D46A7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976" xr2:uid="{03C89AB5-3466-4C93-B69B-4E1CD49D46A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>일일보고</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>비고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메일 서버 구축(postfix)
+메일 서버 작동 원리 공부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spamassassin 적용</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -196,7 +205,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -212,29 +221,32 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,7 +565,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -563,20 +575,22 @@
     <col min="4" max="4" width="15.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
@@ -584,7 +598,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4">
@@ -592,7 +606,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
@@ -600,21 +614,21 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
@@ -623,45 +637,45 @@
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -685,19 +699,23 @@
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A1:C2"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A1:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update report for meeting
</commit_message>
<xml_diff>
--- a/project/spam_mail_detection/주간&일일보고.xlsx
+++ b/project/spam_mail_detection/주간&일일보고.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramie\OneDrive\Documents\learn_programming\project\spam_mail_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749F431A-6FFD-466C-88CD-82A8667DDCE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3196155B-4FCE-4057-B41A-C73031CF0A71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976" xr2:uid="{03C89AB5-3466-4C93-B69B-4E1CD49D46A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>일일보고</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -93,12 +93,17 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>메일 서버 구축(postfix)
-메일 서버 작동 원리 공부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spamassassin 적용</t>
+    <t xml:space="preserve"> - 메일 서버 구축(postfix)
+ - 메일 서버 작동 원리 공부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> - postfix 수신 문제 해결과 spamassassin 연결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> - postfix 수신 문제 해결과 spamassassin 적용
+ - 스팸메일 적용 가능한 데이터셋 탐색</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -205,19 +210,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -227,26 +226,35 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,7 +573,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -576,21 +584,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
@@ -598,15 +606,15 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>44450</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
@@ -614,108 +622,122 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="1"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="1"/>
+      <c r="B12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
     </row>
     <row r="16" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="76.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="1"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" ht="76.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" ht="76.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1"/>
+      <c r="C19" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:D2"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A1:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>